<commit_message>
first run March 2020 data.
</commit_message>
<xml_diff>
--- a/data/First Pass Acceptance_Wiesbaden.xlsx
+++ b/data/First Pass Acceptance_Wiesbaden.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\firstPassAcceptance\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CEE8F69-540C-484B-BE01-7CB3EED48AD5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CD2108-69BA-48A3-BADF-90A479D37B9C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="1590" windowWidth="18900" windowHeight="11055" activeTab="2" xr2:uid="{203EF309-F09C-46D6-B42C-975B3263EA61}"/>
+    <workbookView xWindow="780" yWindow="0" windowWidth="23280" windowHeight="15600" activeTab="2" xr2:uid="{203EF309-F09C-46D6-B42C-975B3263EA61}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ACR!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FPA!$A$1:$J$132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FPA!$A$1:$J$188</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1523" uniqueCount="213">
   <si>
     <t>SQA</t>
   </si>
@@ -539,6 +539,144 @@
   </si>
   <si>
     <t>M1900012</t>
+  </si>
+  <si>
+    <t>Release 01.78.00</t>
+  </si>
+  <si>
+    <t>ZARA</t>
+  </si>
+  <si>
+    <t>L1900290</t>
+  </si>
+  <si>
+    <t>Release 01.80.00</t>
+  </si>
+  <si>
+    <t>Release 01.79.00</t>
+  </si>
+  <si>
+    <t>Wrong SCR</t>
+  </si>
+  <si>
+    <t>Wrong libraries</t>
+  </si>
+  <si>
+    <t>Missing entry</t>
+  </si>
+  <si>
+    <t>Missing, wrong references to URS.</t>
+  </si>
+  <si>
+    <t>REA</t>
+  </si>
+  <si>
+    <t>GIM</t>
+  </si>
+  <si>
+    <t>Missing, wrong references to TP.</t>
+  </si>
+  <si>
+    <t>L1900194</t>
+  </si>
+  <si>
+    <t>Release 01.05.01</t>
+  </si>
+  <si>
+    <t>AQC VERA</t>
+  </si>
+  <si>
+    <t>Offline review. Structure and paths incorrect, requirements contents not matching original</t>
+  </si>
+  <si>
+    <t>Release 02.2x.xx</t>
+  </si>
+  <si>
+    <t>Offline review. Contents need to be adapted to reflect usage of AQC VERA.</t>
+  </si>
+  <si>
+    <t>Offline review. Failure modes and causes need to be corrected.</t>
+  </si>
+  <si>
+    <t>Offline review. Mitigations need to be mapped to requirements.</t>
+  </si>
+  <si>
+    <t>Offline review. AQC090504.A Attachment C no longer exists.</t>
+  </si>
+  <si>
+    <t>Offline review. Tracing needs rework.</t>
+  </si>
+  <si>
+    <t>Offline review.</t>
+  </si>
+  <si>
+    <t>AQC VERA (Base)</t>
+  </si>
+  <si>
+    <t>AQC VERA (Outgoing)</t>
+  </si>
+  <si>
+    <t>AQC VERA (WebApp)</t>
+  </si>
+  <si>
+    <t>AQC VERA (Pricing)</t>
+  </si>
+  <si>
+    <t>Object list incomplete and incorrect. Requires Impact Anaylsis update.</t>
+  </si>
+  <si>
+    <t>Incorrect document used.</t>
+  </si>
+  <si>
+    <t>TP03</t>
+  </si>
+  <si>
+    <t>Copy-paste errors in comments of unexecuted steps.</t>
+  </si>
+  <si>
+    <t>BIA section incorrect</t>
+  </si>
+  <si>
+    <t>A2000019</t>
+  </si>
+  <si>
+    <t>Coment missing</t>
+  </si>
+  <si>
+    <t>Tracing is incomplete</t>
+  </si>
+  <si>
+    <t>LAG</t>
+  </si>
+  <si>
+    <t>Data review section incorrect, BIA section incorrect</t>
+  </si>
+  <si>
+    <t>Release 02.22.00</t>
+  </si>
+  <si>
+    <t>A2000031</t>
+  </si>
+  <si>
+    <t>Outgoing</t>
+  </si>
+  <si>
+    <t>TP69</t>
+  </si>
+  <si>
+    <t>Deliverables tailoring justifications insufficient, documentation impact section incorrect</t>
+  </si>
+  <si>
+    <t>Approver and project roles incorrectly defined</t>
+  </si>
+  <si>
+    <t>Traceability information incomplete</t>
+  </si>
+  <si>
+    <t>Test steps incomplete</t>
+  </si>
+  <si>
+    <t>Unit definitions missing</t>
   </si>
 </sst>
 </file>
@@ -548,7 +686,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,6 +698,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1390,11 +1534,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D811D2-7FE2-4400-8864-3E57D05FCB66}">
-  <dimension ref="A1:J132"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A209" sqref="A209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4878,31 +5022,25 @@
         <v>1</v>
       </c>
       <c r="B123" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="C123" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D123" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
       <c r="E123">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F123" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
       <c r="G123" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H123" s="4">
-        <v>43887</v>
-      </c>
-      <c r="I123" t="s">
-        <v>15</v>
-      </c>
-      <c r="J123" t="s">
-        <v>150</v>
+        <v>43886</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
@@ -4925,11 +5063,17 @@
         <v>23</v>
       </c>
       <c r="G124" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H124" s="4">
         <v>43887</v>
       </c>
+      <c r="I124" t="s">
+        <v>15</v>
+      </c>
+      <c r="J124" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -4942,16 +5086,16 @@
         <v>85</v>
       </c>
       <c r="D125" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="E125">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F125" t="s">
         <v>23</v>
       </c>
       <c r="G125" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H125" s="4">
         <v>43887</v>
@@ -4968,13 +5112,13 @@
         <v>85</v>
       </c>
       <c r="D126" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E126">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F126" t="s">
-        <v>109</v>
+        <v>23</v>
       </c>
       <c r="G126" t="s">
         <v>31</v>
@@ -4994,26 +5138,20 @@
         <v>85</v>
       </c>
       <c r="D127" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E127">
         <v>1</v>
       </c>
       <c r="F127" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="G127" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H127" s="4">
         <v>43887</v>
       </c>
-      <c r="I127" t="s">
-        <v>15</v>
-      </c>
-      <c r="J127" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
@@ -5035,13 +5173,19 @@
         <v>23</v>
       </c>
       <c r="G128" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H128" s="4">
         <v>43887</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128" t="s">
+        <v>15</v>
+      </c>
+      <c r="J128" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>1</v>
       </c>
@@ -5052,48 +5196,48 @@
         <v>85</v>
       </c>
       <c r="D129" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E129">
         <v>1</v>
       </c>
       <c r="F129" t="s">
-        <v>165</v>
+        <v>23</v>
       </c>
       <c r="G129" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H129" s="4">
         <v>43887</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B130" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="C130" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D130" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E130">
         <v>1</v>
       </c>
       <c r="F130" t="s">
-        <v>23</v>
+        <v>165</v>
       </c>
       <c r="G130" t="s">
         <v>31</v>
       </c>
       <c r="H130" s="4">
-        <v>43888</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43887</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>2</v>
       </c>
@@ -5119,44 +5263,2249 @@
         <v>43888</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B132" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
       <c r="C132" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D132" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E132">
         <v>1</v>
       </c>
       <c r="F132" t="s">
-        <v>113</v>
+        <v>23</v>
       </c>
       <c r="G132" t="s">
         <v>31</v>
       </c>
       <c r="H132" s="4">
+        <v>43888</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>1</v>
+      </c>
+      <c r="B133" t="s">
+        <v>155</v>
+      </c>
+      <c r="C133" t="s">
+        <v>85</v>
+      </c>
+      <c r="D133" t="s">
+        <v>69</v>
+      </c>
+      <c r="E133">
+        <v>1</v>
+      </c>
+      <c r="F133" t="s">
+        <v>113</v>
+      </c>
+      <c r="G133" t="s">
+        <v>31</v>
+      </c>
+      <c r="H133" s="4">
         <v>43889</v>
       </c>
     </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>1</v>
+      </c>
+      <c r="B134" t="s">
+        <v>180</v>
+      </c>
+      <c r="C134" t="s">
+        <v>83</v>
+      </c>
+      <c r="D134" t="s">
+        <v>52</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+      <c r="F134" t="s">
+        <v>181</v>
+      </c>
+      <c r="G134" t="s">
+        <v>30</v>
+      </c>
+      <c r="H134" s="4">
+        <v>43889</v>
+      </c>
+      <c r="I134" t="s">
+        <v>22</v>
+      </c>
+      <c r="J134" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>1</v>
+      </c>
+      <c r="B135" t="s">
+        <v>180</v>
+      </c>
+      <c r="C135" t="s">
+        <v>83</v>
+      </c>
+      <c r="D135" t="s">
+        <v>14</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+      <c r="F135" t="s">
+        <v>181</v>
+      </c>
+      <c r="G135" t="s">
+        <v>30</v>
+      </c>
+      <c r="H135" s="4">
+        <v>43892</v>
+      </c>
+      <c r="I135" t="s">
+        <v>22</v>
+      </c>
+      <c r="J135" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>1</v>
+      </c>
+      <c r="B136" t="s">
+        <v>180</v>
+      </c>
+      <c r="C136" t="s">
+        <v>83</v>
+      </c>
+      <c r="D136" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="F136" t="s">
+        <v>181</v>
+      </c>
+      <c r="G136" t="s">
+        <v>30</v>
+      </c>
+      <c r="H136" s="4">
+        <v>43894</v>
+      </c>
+      <c r="I136" t="s">
+        <v>19</v>
+      </c>
+      <c r="J136" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>1</v>
+      </c>
+      <c r="B137" t="s">
+        <v>180</v>
+      </c>
+      <c r="C137" t="s">
+        <v>83</v>
+      </c>
+      <c r="D137" t="s">
+        <v>49</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="F137" t="s">
+        <v>181</v>
+      </c>
+      <c r="G137" t="s">
+        <v>30</v>
+      </c>
+      <c r="H137" s="4">
+        <v>43895</v>
+      </c>
+      <c r="I137" t="s">
+        <v>15</v>
+      </c>
+      <c r="J137" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>2</v>
+      </c>
+      <c r="B138" t="s">
+        <v>167</v>
+      </c>
+      <c r="C138" t="s">
+        <v>92</v>
+      </c>
+      <c r="D138" t="s">
+        <v>51</v>
+      </c>
+      <c r="E138">
+        <v>2</v>
+      </c>
+      <c r="F138" t="s">
+        <v>23</v>
+      </c>
+      <c r="G138" t="s">
+        <v>31</v>
+      </c>
+      <c r="H138" s="4">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" t="s">
+        <v>167</v>
+      </c>
+      <c r="C139" t="s">
+        <v>92</v>
+      </c>
+      <c r="D139" t="s">
+        <v>68</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+      <c r="F139" t="s">
+        <v>23</v>
+      </c>
+      <c r="G139" t="s">
+        <v>31</v>
+      </c>
+      <c r="H139" s="4">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>2</v>
+      </c>
+      <c r="B140" t="s">
+        <v>167</v>
+      </c>
+      <c r="C140" t="s">
+        <v>92</v>
+      </c>
+      <c r="D140" t="s">
+        <v>66</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140" t="s">
+        <v>23</v>
+      </c>
+      <c r="G140" t="s">
+        <v>31</v>
+      </c>
+      <c r="H140" s="4">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" t="s">
+        <v>167</v>
+      </c>
+      <c r="C141" t="s">
+        <v>92</v>
+      </c>
+      <c r="D141" t="s">
+        <v>76</v>
+      </c>
+      <c r="E141">
+        <v>40</v>
+      </c>
+      <c r="F141" t="s">
+        <v>168</v>
+      </c>
+      <c r="G141" t="s">
+        <v>31</v>
+      </c>
+      <c r="H141" s="4">
+        <v>43900</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>1</v>
+      </c>
+      <c r="B142" t="s">
+        <v>180</v>
+      </c>
+      <c r="C142" t="s">
+        <v>83</v>
+      </c>
+      <c r="D142" t="s">
+        <v>14</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+      <c r="F142" t="s">
+        <v>181</v>
+      </c>
+      <c r="G142" t="s">
+        <v>30</v>
+      </c>
+      <c r="H142" s="4">
+        <v>43901</v>
+      </c>
+      <c r="I142" t="s">
+        <v>22</v>
+      </c>
+      <c r="J142" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>2</v>
+      </c>
+      <c r="B143" t="s">
+        <v>167</v>
+      </c>
+      <c r="C143" t="s">
+        <v>92</v>
+      </c>
+      <c r="D143" t="s">
+        <v>69</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143" t="s">
+        <v>109</v>
+      </c>
+      <c r="G143" t="s">
+        <v>31</v>
+      </c>
+      <c r="H143" s="4">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>1</v>
+      </c>
+      <c r="B144" t="s">
+        <v>180</v>
+      </c>
+      <c r="C144" t="s">
+        <v>83</v>
+      </c>
+      <c r="D144" t="s">
+        <v>73</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144" t="s">
+        <v>181</v>
+      </c>
+      <c r="G144" t="s">
+        <v>30</v>
+      </c>
+      <c r="H144" s="4">
+        <v>43902</v>
+      </c>
+      <c r="I144" t="s">
+        <v>22</v>
+      </c>
+      <c r="J144" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>1</v>
+      </c>
+      <c r="B145" t="s">
+        <v>180</v>
+      </c>
+      <c r="C145" t="s">
+        <v>83</v>
+      </c>
+      <c r="D145" t="s">
+        <v>55</v>
+      </c>
+      <c r="E145">
+        <v>1</v>
+      </c>
+      <c r="F145" t="s">
+        <v>181</v>
+      </c>
+      <c r="G145" t="s">
+        <v>30</v>
+      </c>
+      <c r="H145" s="4">
+        <v>43902</v>
+      </c>
+      <c r="I145" t="s">
+        <v>22</v>
+      </c>
+      <c r="J145" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>2</v>
+      </c>
+      <c r="B146" t="s">
+        <v>167</v>
+      </c>
+      <c r="C146" t="s">
+        <v>92</v>
+      </c>
+      <c r="D146" t="s">
+        <v>7</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+      <c r="F146" t="s">
+        <v>23</v>
+      </c>
+      <c r="G146" t="s">
+        <v>31</v>
+      </c>
+      <c r="H146" s="4">
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>2</v>
+      </c>
+      <c r="B147" t="s">
+        <v>167</v>
+      </c>
+      <c r="C147" t="s">
+        <v>92</v>
+      </c>
+      <c r="D147" t="s">
+        <v>71</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+      <c r="F147" t="s">
+        <v>23</v>
+      </c>
+      <c r="G147" t="s">
+        <v>31</v>
+      </c>
+      <c r="H147" s="4">
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>2</v>
+      </c>
+      <c r="B148" t="s">
+        <v>167</v>
+      </c>
+      <c r="C148" t="s">
+        <v>92</v>
+      </c>
+      <c r="D148" t="s">
+        <v>67</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="F148" t="s">
+        <v>23</v>
+      </c>
+      <c r="G148" t="s">
+        <v>31</v>
+      </c>
+      <c r="H148" s="4">
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>1</v>
+      </c>
+      <c r="B149" t="s">
+        <v>180</v>
+      </c>
+      <c r="C149" t="s">
+        <v>83</v>
+      </c>
+      <c r="D149" t="s">
+        <v>55</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149" t="s">
+        <v>181</v>
+      </c>
+      <c r="G149" t="s">
+        <v>30</v>
+      </c>
+      <c r="H149" s="4">
+        <v>43903</v>
+      </c>
+      <c r="I149" t="s">
+        <v>22</v>
+      </c>
+      <c r="J149" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>1</v>
+      </c>
+      <c r="B150" t="s">
+        <v>180</v>
+      </c>
+      <c r="C150" t="s">
+        <v>83</v>
+      </c>
+      <c r="D150" t="s">
+        <v>14</v>
+      </c>
+      <c r="E150">
+        <v>1</v>
+      </c>
+      <c r="F150" t="s">
+        <v>181</v>
+      </c>
+      <c r="G150" t="s">
+        <v>30</v>
+      </c>
+      <c r="H150" s="4">
+        <v>43903</v>
+      </c>
+      <c r="I150" t="s">
+        <v>22</v>
+      </c>
+      <c r="J150" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>2</v>
+      </c>
+      <c r="B151" t="s">
+        <v>167</v>
+      </c>
+      <c r="C151" t="s">
+        <v>92</v>
+      </c>
+      <c r="D151" t="s">
+        <v>69</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151" t="s">
+        <v>113</v>
+      </c>
+      <c r="G151" t="s">
+        <v>31</v>
+      </c>
+      <c r="H151" s="4">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>2</v>
+      </c>
+      <c r="B152" t="s">
+        <v>167</v>
+      </c>
+      <c r="C152" t="s">
+        <v>92</v>
+      </c>
+      <c r="D152" t="s">
+        <v>48</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+      <c r="F152" t="s">
+        <v>169</v>
+      </c>
+      <c r="G152" t="s">
+        <v>31</v>
+      </c>
+      <c r="H152" s="4">
+        <v>43906</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>1</v>
+      </c>
+      <c r="B153" t="s">
+        <v>180</v>
+      </c>
+      <c r="C153" t="s">
+        <v>83</v>
+      </c>
+      <c r="D153" t="s">
+        <v>78</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+      <c r="F153" t="s">
+        <v>181</v>
+      </c>
+      <c r="G153" t="s">
+        <v>30</v>
+      </c>
+      <c r="H153" s="4">
+        <v>43907</v>
+      </c>
+      <c r="I153" t="s">
+        <v>22</v>
+      </c>
+      <c r="J153" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>1</v>
+      </c>
+      <c r="B154" t="s">
+        <v>180</v>
+      </c>
+      <c r="C154" t="s">
+        <v>83</v>
+      </c>
+      <c r="D154" t="s">
+        <v>77</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+      <c r="F154" t="s">
+        <v>181</v>
+      </c>
+      <c r="G154" t="s">
+        <v>30</v>
+      </c>
+      <c r="H154" s="4">
+        <v>43907</v>
+      </c>
+      <c r="I154" t="s">
+        <v>22</v>
+      </c>
+      <c r="J154" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>2</v>
+      </c>
+      <c r="B155" t="s">
+        <v>170</v>
+      </c>
+      <c r="C155" t="s">
+        <v>92</v>
+      </c>
+      <c r="D155" t="s">
+        <v>51</v>
+      </c>
+      <c r="E155">
+        <v>2</v>
+      </c>
+      <c r="F155" t="s">
+        <v>23</v>
+      </c>
+      <c r="G155" t="s">
+        <v>30</v>
+      </c>
+      <c r="H155" s="4">
+        <v>43908</v>
+      </c>
+      <c r="I155" t="s">
+        <v>15</v>
+      </c>
+      <c r="J155" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>1</v>
+      </c>
+      <c r="B156" t="s">
+        <v>140</v>
+      </c>
+      <c r="C156" t="s">
+        <v>90</v>
+      </c>
+      <c r="D156" t="s">
+        <v>68</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+      <c r="F156" t="s">
+        <v>23</v>
+      </c>
+      <c r="G156" t="s">
+        <v>29</v>
+      </c>
+      <c r="H156" s="4">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>2</v>
+      </c>
+      <c r="B157" t="s">
+        <v>171</v>
+      </c>
+      <c r="C157" t="s">
+        <v>92</v>
+      </c>
+      <c r="D157" t="s">
+        <v>63</v>
+      </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
+      <c r="F157" t="s">
+        <v>23</v>
+      </c>
+      <c r="G157" t="s">
+        <v>31</v>
+      </c>
+      <c r="H157" s="4">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>2</v>
+      </c>
+      <c r="B158" t="s">
+        <v>171</v>
+      </c>
+      <c r="C158" t="s">
+        <v>92</v>
+      </c>
+      <c r="D158" t="s">
+        <v>51</v>
+      </c>
+      <c r="E158">
+        <v>2</v>
+      </c>
+      <c r="F158" t="s">
+        <v>23</v>
+      </c>
+      <c r="G158" t="s">
+        <v>30</v>
+      </c>
+      <c r="H158" s="4">
+        <v>43909</v>
+      </c>
+      <c r="I158" t="s">
+        <v>15</v>
+      </c>
+      <c r="J158" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>2</v>
+      </c>
+      <c r="B159" t="s">
+        <v>171</v>
+      </c>
+      <c r="C159" t="s">
+        <v>92</v>
+      </c>
+      <c r="D159" t="s">
+        <v>51</v>
+      </c>
+      <c r="E159">
+        <v>3</v>
+      </c>
+      <c r="F159" t="s">
+        <v>23</v>
+      </c>
+      <c r="G159" t="s">
+        <v>30</v>
+      </c>
+      <c r="H159" s="4">
+        <v>43909</v>
+      </c>
+      <c r="I159" t="s">
+        <v>15</v>
+      </c>
+      <c r="J159" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>2</v>
+      </c>
+      <c r="B160" t="s">
+        <v>171</v>
+      </c>
+      <c r="C160" t="s">
+        <v>92</v>
+      </c>
+      <c r="D160" t="s">
+        <v>51</v>
+      </c>
+      <c r="E160">
+        <v>4</v>
+      </c>
+      <c r="F160" t="s">
+        <v>23</v>
+      </c>
+      <c r="G160" t="s">
+        <v>30</v>
+      </c>
+      <c r="H160" s="4">
+        <v>43909</v>
+      </c>
+      <c r="I160" t="s">
+        <v>15</v>
+      </c>
+      <c r="J160" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>2</v>
+      </c>
+      <c r="B161" t="s">
+        <v>170</v>
+      </c>
+      <c r="C161" t="s">
+        <v>92</v>
+      </c>
+      <c r="D161" t="s">
+        <v>51</v>
+      </c>
+      <c r="E161">
+        <v>2</v>
+      </c>
+      <c r="F161" t="s">
+        <v>23</v>
+      </c>
+      <c r="G161" t="s">
+        <v>29</v>
+      </c>
+      <c r="H161" s="4">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>2</v>
+      </c>
+      <c r="B162" t="s">
+        <v>171</v>
+      </c>
+      <c r="C162" t="s">
+        <v>92</v>
+      </c>
+      <c r="D162" t="s">
+        <v>68</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+      <c r="F162" t="s">
+        <v>23</v>
+      </c>
+      <c r="G162" t="s">
+        <v>31</v>
+      </c>
+      <c r="H162" s="4">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>1</v>
+      </c>
+      <c r="B163" t="s">
+        <v>183</v>
+      </c>
+      <c r="C163" t="s">
+        <v>46</v>
+      </c>
+      <c r="D163" t="s">
+        <v>14</v>
+      </c>
+      <c r="E163">
+        <v>1</v>
+      </c>
+      <c r="F163" t="s">
+        <v>190</v>
+      </c>
+      <c r="G163" t="s">
+        <v>30</v>
+      </c>
+      <c r="H163" s="4">
+        <v>43913</v>
+      </c>
+      <c r="I163" t="s">
+        <v>22</v>
+      </c>
+      <c r="J163" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>1</v>
+      </c>
+      <c r="B164" t="s">
+        <v>140</v>
+      </c>
+      <c r="C164" t="s">
+        <v>90</v>
+      </c>
+      <c r="D164" t="s">
+        <v>7</v>
+      </c>
+      <c r="E164">
+        <v>11</v>
+      </c>
+      <c r="F164" t="s">
+        <v>23</v>
+      </c>
+      <c r="G164" t="s">
+        <v>30</v>
+      </c>
+      <c r="H164" s="4">
+        <v>43913</v>
+      </c>
+      <c r="I164" t="s">
+        <v>22</v>
+      </c>
+      <c r="J164" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>1</v>
+      </c>
+      <c r="B165" t="s">
+        <v>140</v>
+      </c>
+      <c r="C165" t="s">
+        <v>90</v>
+      </c>
+      <c r="D165" t="s">
+        <v>69</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+      <c r="F165" t="s">
+        <v>109</v>
+      </c>
+      <c r="G165" t="s">
+        <v>30</v>
+      </c>
+      <c r="H165" s="4">
+        <v>43913</v>
+      </c>
+      <c r="J165" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>1</v>
+      </c>
+      <c r="B166" t="s">
+        <v>140</v>
+      </c>
+      <c r="C166" t="s">
+        <v>90</v>
+      </c>
+      <c r="D166" t="s">
+        <v>69</v>
+      </c>
+      <c r="E166">
+        <v>1</v>
+      </c>
+      <c r="F166" t="s">
+        <v>109</v>
+      </c>
+      <c r="G166" t="s">
+        <v>29</v>
+      </c>
+      <c r="H166" s="4">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>2</v>
+      </c>
+      <c r="B167" t="s">
+        <v>171</v>
+      </c>
+      <c r="C167" t="s">
+        <v>92</v>
+      </c>
+      <c r="D167" t="s">
+        <v>66</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167" t="s">
+        <v>23</v>
+      </c>
+      <c r="G167" t="s">
+        <v>30</v>
+      </c>
+      <c r="H167" s="4">
+        <v>43913</v>
+      </c>
+      <c r="I167" t="s">
+        <v>22</v>
+      </c>
+      <c r="J167" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>1</v>
+      </c>
+      <c r="B168" t="s">
+        <v>183</v>
+      </c>
+      <c r="C168" t="s">
+        <v>46</v>
+      </c>
+      <c r="D168" t="s">
+        <v>14</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+      <c r="F168" t="s">
+        <v>191</v>
+      </c>
+      <c r="G168" t="s">
+        <v>30</v>
+      </c>
+      <c r="H168" s="4">
+        <v>43914</v>
+      </c>
+      <c r="I168" t="s">
+        <v>22</v>
+      </c>
+      <c r="J168" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>2</v>
+      </c>
+      <c r="B169" t="s">
+        <v>171</v>
+      </c>
+      <c r="C169" t="s">
+        <v>92</v>
+      </c>
+      <c r="D169" t="s">
+        <v>51</v>
+      </c>
+      <c r="E169">
+        <v>5</v>
+      </c>
+      <c r="F169" t="s">
+        <v>23</v>
+      </c>
+      <c r="G169" t="s">
+        <v>29</v>
+      </c>
+      <c r="H169" s="4">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>2</v>
+      </c>
+      <c r="B170" t="s">
+        <v>171</v>
+      </c>
+      <c r="C170" t="s">
+        <v>92</v>
+      </c>
+      <c r="D170" t="s">
+        <v>66</v>
+      </c>
+      <c r="E170">
+        <v>2</v>
+      </c>
+      <c r="F170" t="s">
+        <v>23</v>
+      </c>
+      <c r="G170" t="s">
+        <v>29</v>
+      </c>
+      <c r="H170" s="4">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>2</v>
+      </c>
+      <c r="B171" t="s">
+        <v>171</v>
+      </c>
+      <c r="C171" t="s">
+        <v>92</v>
+      </c>
+      <c r="D171" t="s">
+        <v>76</v>
+      </c>
+      <c r="E171">
+        <v>14</v>
+      </c>
+      <c r="F171" t="s">
+        <v>176</v>
+      </c>
+      <c r="G171" t="s">
+        <v>31</v>
+      </c>
+      <c r="H171" s="4">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>2</v>
+      </c>
+      <c r="B172" t="s">
+        <v>171</v>
+      </c>
+      <c r="C172" t="s">
+        <v>92</v>
+      </c>
+      <c r="D172" t="s">
+        <v>76</v>
+      </c>
+      <c r="E172">
+        <v>26</v>
+      </c>
+      <c r="F172" t="s">
+        <v>177</v>
+      </c>
+      <c r="G172" t="s">
+        <v>30</v>
+      </c>
+      <c r="H172" s="4">
+        <v>43914</v>
+      </c>
+      <c r="I172" t="s">
+        <v>22</v>
+      </c>
+      <c r="J172" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>2</v>
+      </c>
+      <c r="B173" t="s">
+        <v>171</v>
+      </c>
+      <c r="C173" t="s">
+        <v>92</v>
+      </c>
+      <c r="D173" t="s">
+        <v>76</v>
+      </c>
+      <c r="E173">
+        <v>26</v>
+      </c>
+      <c r="F173" t="s">
+        <v>177</v>
+      </c>
+      <c r="G173" t="s">
+        <v>29</v>
+      </c>
+      <c r="H173" s="4">
+        <v>43914</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>1</v>
+      </c>
+      <c r="B174" t="s">
+        <v>183</v>
+      </c>
+      <c r="C174" t="s">
+        <v>46</v>
+      </c>
+      <c r="D174" t="s">
+        <v>14</v>
+      </c>
+      <c r="E174">
+        <v>1</v>
+      </c>
+      <c r="F174" t="s">
+        <v>192</v>
+      </c>
+      <c r="G174" t="s">
+        <v>30</v>
+      </c>
+      <c r="H174" s="4">
+        <v>43915</v>
+      </c>
+      <c r="I174" t="s">
+        <v>22</v>
+      </c>
+      <c r="J174" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>1</v>
+      </c>
+      <c r="B175" t="s">
+        <v>183</v>
+      </c>
+      <c r="C175" t="s">
+        <v>46</v>
+      </c>
+      <c r="D175" t="s">
+        <v>14</v>
+      </c>
+      <c r="E175">
+        <v>1</v>
+      </c>
+      <c r="F175" t="s">
+        <v>193</v>
+      </c>
+      <c r="G175" t="s">
+        <v>30</v>
+      </c>
+      <c r="H175" s="4">
+        <v>43915</v>
+      </c>
+      <c r="I175" t="s">
+        <v>22</v>
+      </c>
+      <c r="J175" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>1</v>
+      </c>
+      <c r="B176" t="s">
+        <v>140</v>
+      </c>
+      <c r="C176" t="s">
+        <v>90</v>
+      </c>
+      <c r="D176" t="s">
+        <v>7</v>
+      </c>
+      <c r="E176">
+        <v>11</v>
+      </c>
+      <c r="F176" t="s">
+        <v>23</v>
+      </c>
+      <c r="G176" t="s">
+        <v>29</v>
+      </c>
+      <c r="H176" s="4">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>1</v>
+      </c>
+      <c r="B177" t="s">
+        <v>140</v>
+      </c>
+      <c r="C177" t="s">
+        <v>90</v>
+      </c>
+      <c r="D177" t="s">
+        <v>51</v>
+      </c>
+      <c r="E177">
+        <v>2</v>
+      </c>
+      <c r="F177" t="s">
+        <v>23</v>
+      </c>
+      <c r="G177" t="s">
+        <v>31</v>
+      </c>
+      <c r="H177" s="4">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>2</v>
+      </c>
+      <c r="B178" t="s">
+        <v>171</v>
+      </c>
+      <c r="C178" t="s">
+        <v>92</v>
+      </c>
+      <c r="D178" t="s">
+        <v>7</v>
+      </c>
+      <c r="E178">
+        <v>1</v>
+      </c>
+      <c r="F178" t="s">
+        <v>23</v>
+      </c>
+      <c r="G178" t="s">
+        <v>31</v>
+      </c>
+      <c r="H178" s="4">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>2</v>
+      </c>
+      <c r="B179" t="s">
+        <v>171</v>
+      </c>
+      <c r="C179" t="s">
+        <v>92</v>
+      </c>
+      <c r="D179" t="s">
+        <v>68</v>
+      </c>
+      <c r="E179">
+        <v>2</v>
+      </c>
+      <c r="F179" t="s">
+        <v>23</v>
+      </c>
+      <c r="G179" t="s">
+        <v>31</v>
+      </c>
+      <c r="H179" s="4">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>2</v>
+      </c>
+      <c r="B180" t="s">
+        <v>171</v>
+      </c>
+      <c r="C180" t="s">
+        <v>92</v>
+      </c>
+      <c r="D180" t="s">
+        <v>69</v>
+      </c>
+      <c r="E180">
+        <v>1</v>
+      </c>
+      <c r="F180" t="s">
+        <v>109</v>
+      </c>
+      <c r="G180" t="s">
+        <v>31</v>
+      </c>
+      <c r="H180" s="4">
+        <v>43915</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>2</v>
+      </c>
+      <c r="B181" t="s">
+        <v>171</v>
+      </c>
+      <c r="C181" t="s">
+        <v>92</v>
+      </c>
+      <c r="D181" t="s">
+        <v>71</v>
+      </c>
+      <c r="E181">
+        <v>1</v>
+      </c>
+      <c r="F181" t="s">
+        <v>23</v>
+      </c>
+      <c r="G181" t="s">
+        <v>31</v>
+      </c>
+      <c r="H181" s="4">
+        <v>43916</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>2</v>
+      </c>
+      <c r="B182" t="s">
+        <v>171</v>
+      </c>
+      <c r="C182" t="s">
+        <v>92</v>
+      </c>
+      <c r="D182" t="s">
+        <v>67</v>
+      </c>
+      <c r="E182">
+        <v>1</v>
+      </c>
+      <c r="F182" t="s">
+        <v>23</v>
+      </c>
+      <c r="G182" t="s">
+        <v>31</v>
+      </c>
+      <c r="H182" s="4">
+        <v>43916</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>1</v>
+      </c>
+      <c r="B183" t="s">
+        <v>140</v>
+      </c>
+      <c r="C183" t="s">
+        <v>90</v>
+      </c>
+      <c r="D183" t="s">
+        <v>69</v>
+      </c>
+      <c r="E183">
+        <v>1</v>
+      </c>
+      <c r="F183" t="s">
+        <v>113</v>
+      </c>
+      <c r="G183" t="s">
+        <v>31</v>
+      </c>
+      <c r="H183" s="4">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>1</v>
+      </c>
+      <c r="B184" t="s">
+        <v>140</v>
+      </c>
+      <c r="C184" t="s">
+        <v>90</v>
+      </c>
+      <c r="D184" t="s">
+        <v>71</v>
+      </c>
+      <c r="E184">
+        <v>1</v>
+      </c>
+      <c r="F184" t="s">
+        <v>23</v>
+      </c>
+      <c r="G184" t="s">
+        <v>30</v>
+      </c>
+      <c r="H184" s="4">
+        <v>43917</v>
+      </c>
+      <c r="I184" t="s">
+        <v>15</v>
+      </c>
+      <c r="J184" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>1</v>
+      </c>
+      <c r="B185" t="s">
+        <v>140</v>
+      </c>
+      <c r="C185" t="s">
+        <v>90</v>
+      </c>
+      <c r="D185" t="s">
+        <v>71</v>
+      </c>
+      <c r="E185">
+        <v>1</v>
+      </c>
+      <c r="F185" t="s">
+        <v>23</v>
+      </c>
+      <c r="G185" t="s">
+        <v>29</v>
+      </c>
+      <c r="H185" s="4">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>1</v>
+      </c>
+      <c r="B186" t="s">
+        <v>140</v>
+      </c>
+      <c r="C186" t="s">
+        <v>90</v>
+      </c>
+      <c r="D186" t="s">
+        <v>71</v>
+      </c>
+      <c r="E186">
+        <v>1</v>
+      </c>
+      <c r="F186" t="s">
+        <v>23</v>
+      </c>
+      <c r="G186" t="s">
+        <v>30</v>
+      </c>
+      <c r="H186" s="4">
+        <v>43917</v>
+      </c>
+      <c r="I186" t="s">
+        <v>15</v>
+      </c>
+      <c r="J186" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>1</v>
+      </c>
+      <c r="B187" t="s">
+        <v>140</v>
+      </c>
+      <c r="C187" t="s">
+        <v>90</v>
+      </c>
+      <c r="D187" t="s">
+        <v>71</v>
+      </c>
+      <c r="E187">
+        <v>1</v>
+      </c>
+      <c r="F187" t="s">
+        <v>23</v>
+      </c>
+      <c r="G187" t="s">
+        <v>29</v>
+      </c>
+      <c r="H187" s="4">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>1</v>
+      </c>
+      <c r="B188" t="s">
+        <v>140</v>
+      </c>
+      <c r="C188" t="s">
+        <v>90</v>
+      </c>
+      <c r="D188" t="s">
+        <v>67</v>
+      </c>
+      <c r="E188">
+        <v>1</v>
+      </c>
+      <c r="F188" t="s">
+        <v>196</v>
+      </c>
+      <c r="G188" t="s">
+        <v>30</v>
+      </c>
+      <c r="H188" s="4">
+        <v>43917</v>
+      </c>
+      <c r="I188" t="s">
+        <v>22</v>
+      </c>
+      <c r="J188" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>1</v>
+      </c>
+      <c r="B189" t="s">
+        <v>140</v>
+      </c>
+      <c r="C189" t="s">
+        <v>90</v>
+      </c>
+      <c r="D189" t="s">
+        <v>67</v>
+      </c>
+      <c r="E189">
+        <v>1</v>
+      </c>
+      <c r="F189" t="s">
+        <v>196</v>
+      </c>
+      <c r="G189" t="s">
+        <v>29</v>
+      </c>
+      <c r="H189" s="4">
+        <v>43917</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>1</v>
+      </c>
+      <c r="B190" t="s">
+        <v>204</v>
+      </c>
+      <c r="C190" t="s">
+        <v>46</v>
+      </c>
+      <c r="D190" t="s">
+        <v>48</v>
+      </c>
+      <c r="E190">
+        <v>1</v>
+      </c>
+      <c r="F190" t="s">
+        <v>205</v>
+      </c>
+      <c r="G190" t="s">
+        <v>31</v>
+      </c>
+      <c r="H190" s="4">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>1</v>
+      </c>
+      <c r="B191" t="s">
+        <v>204</v>
+      </c>
+      <c r="C191" t="s">
+        <v>46</v>
+      </c>
+      <c r="D191" t="s">
+        <v>52</v>
+      </c>
+      <c r="E191">
+        <v>1</v>
+      </c>
+      <c r="F191" t="s">
+        <v>23</v>
+      </c>
+      <c r="G191" t="s">
+        <v>30</v>
+      </c>
+      <c r="H191" s="4">
+        <v>43920</v>
+      </c>
+      <c r="I191" t="s">
+        <v>15</v>
+      </c>
+      <c r="J191" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>2</v>
+      </c>
+      <c r="B192" t="s">
+        <v>171</v>
+      </c>
+      <c r="C192" t="s">
+        <v>92</v>
+      </c>
+      <c r="D192" t="s">
+        <v>69</v>
+      </c>
+      <c r="E192">
+        <v>1</v>
+      </c>
+      <c r="F192" t="s">
+        <v>113</v>
+      </c>
+      <c r="G192" t="s">
+        <v>30</v>
+      </c>
+      <c r="H192" s="4">
+        <v>43920</v>
+      </c>
+      <c r="I192" t="s">
+        <v>15</v>
+      </c>
+      <c r="J192" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>2</v>
+      </c>
+      <c r="B193" t="s">
+        <v>171</v>
+      </c>
+      <c r="C193" t="s">
+        <v>92</v>
+      </c>
+      <c r="D193" t="s">
+        <v>69</v>
+      </c>
+      <c r="E193">
+        <v>1</v>
+      </c>
+      <c r="F193" t="s">
+        <v>113</v>
+      </c>
+      <c r="G193" t="s">
+        <v>29</v>
+      </c>
+      <c r="H193" s="4">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>2</v>
+      </c>
+      <c r="B194" t="s">
+        <v>171</v>
+      </c>
+      <c r="C194" t="s">
+        <v>92</v>
+      </c>
+      <c r="D194" t="s">
+        <v>48</v>
+      </c>
+      <c r="E194">
+        <v>1</v>
+      </c>
+      <c r="F194" t="s">
+        <v>179</v>
+      </c>
+      <c r="G194" t="s">
+        <v>31</v>
+      </c>
+      <c r="H194" s="4">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>2</v>
+      </c>
+      <c r="B195" t="s">
+        <v>170</v>
+      </c>
+      <c r="C195" t="s">
+        <v>92</v>
+      </c>
+      <c r="D195" t="s">
+        <v>66</v>
+      </c>
+      <c r="E195">
+        <v>2</v>
+      </c>
+      <c r="F195" t="s">
+        <v>23</v>
+      </c>
+      <c r="G195" t="s">
+        <v>30</v>
+      </c>
+      <c r="H195" s="4">
+        <v>43920</v>
+      </c>
+      <c r="I195" t="s">
+        <v>22</v>
+      </c>
+      <c r="J195" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>2</v>
+      </c>
+      <c r="B196" t="s">
+        <v>170</v>
+      </c>
+      <c r="C196" t="s">
+        <v>92</v>
+      </c>
+      <c r="D196" t="s">
+        <v>76</v>
+      </c>
+      <c r="E196">
+        <v>6</v>
+      </c>
+      <c r="F196" t="s">
+        <v>202</v>
+      </c>
+      <c r="G196" t="s">
+        <v>30</v>
+      </c>
+      <c r="H196" s="4">
+        <v>43920</v>
+      </c>
+      <c r="I196" t="s">
+        <v>22</v>
+      </c>
+      <c r="J196" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>1</v>
+      </c>
+      <c r="B197" t="s">
+        <v>204</v>
+      </c>
+      <c r="C197" t="s">
+        <v>46</v>
+      </c>
+      <c r="D197" t="s">
+        <v>51</v>
+      </c>
+      <c r="E197">
+        <v>1</v>
+      </c>
+      <c r="F197" t="s">
+        <v>23</v>
+      </c>
+      <c r="G197" t="s">
+        <v>30</v>
+      </c>
+      <c r="H197" s="4">
+        <v>43921</v>
+      </c>
+      <c r="I197" t="s">
+        <v>22</v>
+      </c>
+      <c r="J197" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>1</v>
+      </c>
+      <c r="B198" t="s">
+        <v>204</v>
+      </c>
+      <c r="C198" t="s">
+        <v>46</v>
+      </c>
+      <c r="D198" t="s">
+        <v>52</v>
+      </c>
+      <c r="E198">
+        <v>1</v>
+      </c>
+      <c r="F198" t="s">
+        <v>23</v>
+      </c>
+      <c r="G198" t="s">
+        <v>29</v>
+      </c>
+      <c r="H198" s="4">
+        <v>43921</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>1</v>
+      </c>
+      <c r="B199" t="s">
+        <v>204</v>
+      </c>
+      <c r="C199" t="s">
+        <v>46</v>
+      </c>
+      <c r="D199" t="s">
+        <v>66</v>
+      </c>
+      <c r="E199">
+        <v>1</v>
+      </c>
+      <c r="F199" t="s">
+        <v>207</v>
+      </c>
+      <c r="G199" t="s">
+        <v>30</v>
+      </c>
+      <c r="H199" s="4">
+        <v>43921</v>
+      </c>
+      <c r="I199" t="s">
+        <v>15</v>
+      </c>
+      <c r="J199" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>1</v>
+      </c>
+      <c r="B200" t="s">
+        <v>204</v>
+      </c>
+      <c r="C200" t="s">
+        <v>46</v>
+      </c>
+      <c r="D200" t="s">
+        <v>76</v>
+      </c>
+      <c r="E200">
+        <v>26</v>
+      </c>
+      <c r="F200" t="s">
+        <v>206</v>
+      </c>
+      <c r="G200" t="s">
+        <v>30</v>
+      </c>
+      <c r="H200" s="4">
+        <v>43921</v>
+      </c>
+      <c r="I200" t="s">
+        <v>15</v>
+      </c>
+      <c r="J200" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>1</v>
+      </c>
+      <c r="B201" t="s">
+        <v>204</v>
+      </c>
+      <c r="C201" t="s">
+        <v>46</v>
+      </c>
+      <c r="D201" t="s">
+        <v>63</v>
+      </c>
+      <c r="E201">
+        <v>1</v>
+      </c>
+      <c r="F201" t="s">
+        <v>206</v>
+      </c>
+      <c r="G201" t="s">
+        <v>30</v>
+      </c>
+      <c r="H201" s="4">
+        <v>43922</v>
+      </c>
+      <c r="I201" t="s">
+        <v>15</v>
+      </c>
+      <c r="J201" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>1</v>
+      </c>
+      <c r="B202" t="s">
+        <v>204</v>
+      </c>
+      <c r="C202" t="s">
+        <v>46</v>
+      </c>
+      <c r="D202" t="s">
+        <v>63</v>
+      </c>
+      <c r="E202">
+        <v>1</v>
+      </c>
+      <c r="F202" t="s">
+        <v>206</v>
+      </c>
+      <c r="G202" t="s">
+        <v>29</v>
+      </c>
+      <c r="H202" s="4">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>1</v>
+      </c>
+      <c r="B203" t="s">
+        <v>204</v>
+      </c>
+      <c r="C203" t="s">
+        <v>46</v>
+      </c>
+      <c r="D203" t="s">
+        <v>68</v>
+      </c>
+      <c r="E203">
+        <v>1</v>
+      </c>
+      <c r="F203" t="s">
+        <v>23</v>
+      </c>
+      <c r="G203" t="s">
+        <v>31</v>
+      </c>
+      <c r="H203" s="4">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>1</v>
+      </c>
+      <c r="B204" t="s">
+        <v>204</v>
+      </c>
+      <c r="C204" t="s">
+        <v>46</v>
+      </c>
+      <c r="D204" t="s">
+        <v>66</v>
+      </c>
+      <c r="E204">
+        <v>1</v>
+      </c>
+      <c r="F204" t="s">
+        <v>207</v>
+      </c>
+      <c r="G204" t="s">
+        <v>29</v>
+      </c>
+      <c r="H204" s="4">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>1</v>
+      </c>
+      <c r="B205" t="s">
+        <v>204</v>
+      </c>
+      <c r="C205" t="s">
+        <v>46</v>
+      </c>
+      <c r="D205" t="s">
+        <v>7</v>
+      </c>
+      <c r="E205">
+        <v>1</v>
+      </c>
+      <c r="F205" t="s">
+        <v>23</v>
+      </c>
+      <c r="G205" t="s">
+        <v>31</v>
+      </c>
+      <c r="H205" s="4">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>1</v>
+      </c>
+      <c r="B206" t="s">
+        <v>204</v>
+      </c>
+      <c r="C206" t="s">
+        <v>46</v>
+      </c>
+      <c r="D206" t="s">
+        <v>69</v>
+      </c>
+      <c r="E206">
+        <v>1</v>
+      </c>
+      <c r="F206" t="s">
+        <v>109</v>
+      </c>
+      <c r="G206" t="s">
+        <v>31</v>
+      </c>
+      <c r="H206" s="4">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>1</v>
+      </c>
+      <c r="B207" t="s">
+        <v>204</v>
+      </c>
+      <c r="C207" t="s">
+        <v>46</v>
+      </c>
+      <c r="D207" t="s">
+        <v>69</v>
+      </c>
+      <c r="E207">
+        <v>1</v>
+      </c>
+      <c r="F207" t="s">
+        <v>113</v>
+      </c>
+      <c r="G207" t="s">
+        <v>31</v>
+      </c>
+      <c r="H207" s="4">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>1</v>
+      </c>
+      <c r="B208" t="s">
+        <v>204</v>
+      </c>
+      <c r="C208" t="s">
+        <v>46</v>
+      </c>
+      <c r="D208" t="s">
+        <v>71</v>
+      </c>
+      <c r="E208">
+        <v>1</v>
+      </c>
+      <c r="F208" t="s">
+        <v>23</v>
+      </c>
+      <c r="G208" t="s">
+        <v>31</v>
+      </c>
+      <c r="H208" s="4">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>1</v>
+      </c>
+      <c r="B209" t="s">
+        <v>204</v>
+      </c>
+      <c r="C209" t="s">
+        <v>46</v>
+      </c>
+      <c r="D209" t="s">
+        <v>67</v>
+      </c>
+      <c r="E209">
+        <v>1</v>
+      </c>
+      <c r="F209" t="s">
+        <v>207</v>
+      </c>
+      <c r="G209" t="s">
+        <v>31</v>
+      </c>
+      <c r="H209" s="4">
+        <v>43923</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J132" xr:uid="{666A33B2-D072-48D0-88E3-92275EF5620C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J103">
-      <sortCondition ref="H2:H103"/>
-      <sortCondition ref="B2:B103"/>
+  <autoFilter ref="A1:J188" xr:uid="{666A33B2-D072-48D0-88E3-92275EF5620C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J188">
+      <sortCondition ref="H2:H188"/>
+      <sortCondition ref="C2:C188"/>
+      <sortCondition ref="B2:B188"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J129">
-    <sortCondition ref="H2:H129"/>
-    <sortCondition ref="C2:C129"/>
-    <sortCondition ref="D2:D129"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J209">
+    <sortCondition ref="H2:H209"/>
+    <sortCondition ref="C2:C209"/>
+    <sortCondition ref="D2:D209"/>
   </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
reprosedd June 2020 data with New revised wiesbaden data
</commit_message>
<xml_diff>
--- a/data/First Pass Acceptance_Wiesbaden.xlsx
+++ b/data/First Pass Acceptance_Wiesbaden.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\firstPassAcceptance\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E74EFF0-84E8-48C8-8C17-2F536948FCE0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC09B9E-423C-4D31-8ECD-368AD8FA9187}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{203EF309-F09C-46D6-B42C-975B3263EA61}"/>
+    <workbookView xWindow="22530" yWindow="1245" windowWidth="25470" windowHeight="18420" activeTab="2" xr2:uid="{203EF309-F09C-46D6-B42C-975B3263EA61}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ACR!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FPA!$A$1:$J$309</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">FPA!$A$1:$J$396</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2828" uniqueCount="309">
   <si>
     <t>SQA</t>
   </si>
@@ -851,6 +851,120 @@
   </si>
   <si>
     <t>Additional changes required, contents incorrect, tracing is still partially missing</t>
+  </si>
+  <si>
+    <t>FSP</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>Several fields empty</t>
+  </si>
+  <si>
+    <t>Several incorrect references</t>
+  </si>
+  <si>
+    <t>Release 1.1</t>
+  </si>
+  <si>
+    <t>FIIS</t>
+  </si>
+  <si>
+    <t>Several version information mismatches</t>
+  </si>
+  <si>
+    <t>BPO &amp; TR missing</t>
+  </si>
+  <si>
+    <t>WI_C000001</t>
+  </si>
+  <si>
+    <t>WI_C000002</t>
+  </si>
+  <si>
+    <t>WI_L000001</t>
+  </si>
+  <si>
+    <t>Release 9.7</t>
+  </si>
+  <si>
+    <t>MCPR</t>
+  </si>
+  <si>
+    <t>AIR is no longer used, transition to SCR/ACR/IPDR in AQC VERA has concluded</t>
+  </si>
+  <si>
+    <t>Req Coverage missing</t>
+  </si>
+  <si>
+    <t>Release 01.82.00</t>
+  </si>
+  <si>
+    <t>L2000112</t>
+  </si>
+  <si>
+    <t>L2000073</t>
+  </si>
+  <si>
+    <t>L2000066</t>
+  </si>
+  <si>
+    <t>L2000117</t>
+  </si>
+  <si>
+    <t>Release 01.83.00</t>
+  </si>
+  <si>
+    <t>ALC</t>
+  </si>
+  <si>
+    <t>L2000060</t>
+  </si>
+  <si>
+    <t>Release content change</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>Contains several references to AIR and descriptions of the workflows</t>
+  </si>
+  <si>
+    <t>Several trace links missing or incorrect</t>
+  </si>
+  <si>
+    <t>One empty step needs to be deleted</t>
+  </si>
+  <si>
+    <t>Contains reference to eRIM, replace with DLM</t>
+  </si>
+  <si>
+    <t>Incorrrect SPR references, tailoring incorrect, contains reference to eRIM, replace with DLM</t>
+  </si>
+  <si>
+    <t>Rich text filled with redndant information</t>
+  </si>
+  <si>
+    <t>WI_L000002</t>
+  </si>
+  <si>
+    <t>GER42 serial# missing</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>2b</t>
+  </si>
+  <si>
+    <t>Additional code</t>
+  </si>
+  <si>
+    <t>17a</t>
+  </si>
+  <si>
+    <t>17b</t>
   </si>
 </sst>
 </file>
@@ -909,7 +1023,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -921,6 +1035,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1235,7 +1350,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A1818BC-AC9F-4D38-87AF-905538E5415F}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1348,7 +1463,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>84</v>
+        <v>276</v>
       </c>
       <c r="C8" t="s">
         <v>62</v>
@@ -1359,7 +1474,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>85</v>
+        <v>271</v>
       </c>
       <c r="C9" t="s">
         <v>63</v>
@@ -1370,7 +1485,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>91</v>
+        <v>272</v>
       </c>
       <c r="C10" t="s">
         <v>49</v>
@@ -1381,7 +1496,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -1392,7 +1507,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
         <v>51</v>
@@ -1403,7 +1518,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -1414,7 +1529,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
         <v>68</v>
@@ -1425,7 +1540,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
@@ -1436,7 +1551,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -1447,7 +1562,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
         <v>69</v>
@@ -1455,7 +1570,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
         <v>56</v>
@@ -1463,152 +1578,166 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>101</v>
       </c>
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>264</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>53</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>145</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E44">
-    <sortCondition ref="C25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E48">
+    <sortCondition ref="C29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1617,11 +1746,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DAE5DB-E055-4B79-809B-3CC2C4CB7528}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,30 +1799,153 @@
         <v>39</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="7">
+        <v>44019</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="7">
+        <v>44021</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D4" s="7">
+        <v>44022</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D5" s="7">
+        <v>44033</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>281</v>
+      </c>
+      <c r="G6" s="7">
+        <v>44041</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D7" s="7">
+        <v>44041</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D8" s="7">
+        <v>44043</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J1" xr:uid="{3A9C1769-6EE6-49EC-A1F0-37710006E669}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J4">
+    <sortCondition ref="D2:D4"/>
+    <sortCondition ref="B2:B4"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C3C92040-D72E-4EF6-BBC5-6AA8D8595C6E}">
           <x14:formula1>
             <xm:f>Config!$D$2:$D$16</xm:f>
           </x14:formula1>
           <xm:sqref>I2:I1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4260E77A-0060-4AD1-A06E-9DFD65E1B213}">
-          <x14:formula1>
-            <xm:f>Config!$B$2:$B$103</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C1362870-EEE2-41F3-81AD-20771FC144DE}">
-          <x14:formula1>
-            <xm:f>Config!$E$2:$E$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2D2E8A2F-93BE-491B-B991-93FA52D368BA}">
           <x14:formula1>
@@ -1705,7 +1957,13 @@
           <x14:formula1>
             <xm:f>Config!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>H2:H1048576 E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4260E77A-0060-4AD1-A06E-9DFD65E1B213}">
+          <x14:formula1>
+            <xm:f>Config!$B$2:$B$106</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1715,11 +1973,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D811D2-7FE2-4400-8864-3E57D05FCB66}">
-  <dimension ref="A1:J315"/>
+  <dimension ref="A1:J396"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A299" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A316" sqref="A316"/>
+      <pane ySplit="1" topLeftCell="A359" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H364" sqref="H364"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10692,19 +10950,19 @@
     </row>
     <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B313" s="5" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
       <c r="C313" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D313" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E313" s="5">
-        <v>1</v>
+        <v>51</v>
+      </c>
+      <c r="E313" s="5" t="s">
+        <v>260</v>
       </c>
       <c r="F313" s="5" t="s">
         <v>23</v>
@@ -10712,90 +10970,2413 @@
       <c r="G313" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H313" s="4">
-        <v>43999</v>
+      <c r="H313" s="6">
+        <v>43997</v>
       </c>
       <c r="I313" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="J313" s="5" t="s">
-        <v>268</v>
+        <v>294</v>
       </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B314" s="5" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
       <c r="C314" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D314" s="5" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="E314" s="5">
         <v>1</v>
       </c>
       <c r="F314" s="5" t="s">
-        <v>23</v>
+        <v>288</v>
       </c>
       <c r="G314" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H314" s="4">
-        <v>44001</v>
-      </c>
-      <c r="I314" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J314" s="5" t="s">
-        <v>269</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H314" s="6">
+        <v>43997</v>
+      </c>
+      <c r="I314" s="5"/>
+      <c r="J314" s="5"/>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B315" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C315" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D315" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E315" s="5">
+        <v>1</v>
+      </c>
+      <c r="F315" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G315" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H315" s="6">
+        <v>43997</v>
+      </c>
+      <c r="I315" s="5"/>
+      <c r="J315" s="5"/>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A316" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B316" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C316" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D316" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E316" s="5">
+        <v>1</v>
+      </c>
+      <c r="F316" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G316" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H316" s="6">
+        <v>43997</v>
+      </c>
+      <c r="I316" s="5"/>
+      <c r="J316" s="5"/>
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A317" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B317" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C317" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D317" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E317" s="5">
+        <v>49</v>
+      </c>
+      <c r="F317" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G317" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H317" s="6">
+        <v>43997</v>
+      </c>
+      <c r="I317" s="5"/>
+      <c r="J317" s="5"/>
+    </row>
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A318" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B318" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C318" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D318" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E318" s="5">
+        <v>45</v>
+      </c>
+      <c r="F318" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G318" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H318" s="6">
+        <v>43997</v>
+      </c>
+      <c r="I318" s="5"/>
+      <c r="J318" s="5"/>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A319" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B319" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C319" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D319" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E319" s="5">
+        <v>30</v>
+      </c>
+      <c r="F319" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="G319" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H319" s="6">
+        <v>43997</v>
+      </c>
+      <c r="I319" s="5"/>
+      <c r="J319" s="5"/>
+    </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A320" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B320" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="C315" s="5" t="s">
+      <c r="C320" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D315" s="5" t="s">
+      <c r="D320" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E315" s="5">
-        <v>1</v>
-      </c>
-      <c r="F315" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G315" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H315" s="4">
+      <c r="E320" s="5">
+        <v>1</v>
+      </c>
+      <c r="F320" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G320" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H320" s="4">
+        <v>43999</v>
+      </c>
+      <c r="I320" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J320" s="5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A321" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B321" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C321" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D321" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E321" s="5">
+        <v>1</v>
+      </c>
+      <c r="F321" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G321" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H321" s="6">
+        <v>44000</v>
+      </c>
+      <c r="I321" s="5"/>
+      <c r="J321" s="5"/>
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A322" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B322" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C322" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D322" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E322" s="5">
+        <v>2</v>
+      </c>
+      <c r="F322" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G322" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H322" s="6">
+        <v>44000</v>
+      </c>
+      <c r="I322" s="5"/>
+      <c r="J322" s="5"/>
+    </row>
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A323" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B323" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C323" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D323" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E323" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F323" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G323" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H323" s="6">
+        <v>44000</v>
+      </c>
+      <c r="I323" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J323" s="5"/>
+    </row>
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A324" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B324" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C324" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D324" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E324" s="5">
+        <v>1</v>
+      </c>
+      <c r="F324" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G324" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H324" s="4">
+        <v>44001</v>
+      </c>
+      <c r="I324" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J324" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A325" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B325" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C325" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D325" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E325" s="5">
+        <v>1</v>
+      </c>
+      <c r="F325" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G325" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H325" s="6">
+        <v>44001</v>
+      </c>
+      <c r="I325" s="5"/>
+      <c r="J325" s="5"/>
+    </row>
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A326" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B326" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C326" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D326" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E326" s="5">
+        <v>1</v>
+      </c>
+      <c r="F326" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="G326" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H326" s="6">
+        <v>44001</v>
+      </c>
+      <c r="I326" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J326" s="5"/>
+    </row>
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A327" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B327" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C327" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D327" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E327" s="5">
+        <v>1</v>
+      </c>
+      <c r="F327" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G327" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H327" s="6">
+        <v>44001</v>
+      </c>
+      <c r="I327" s="5"/>
+      <c r="J327" s="5"/>
+    </row>
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A328" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B328" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C328" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D328" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E328" s="5">
+        <v>1</v>
+      </c>
+      <c r="F328" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="G328" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H328" s="6">
+        <v>44001</v>
+      </c>
+      <c r="I328" s="5"/>
+      <c r="J328" s="5"/>
+    </row>
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A329" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B329" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C329" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D329" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E329" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F329" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G329" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H329" s="6">
+        <v>44001</v>
+      </c>
+      <c r="I329" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J329" s="5"/>
+    </row>
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A330" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B330" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C330" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D330" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E330" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F330" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G330" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H330" s="6">
+        <v>44001</v>
+      </c>
+      <c r="I330" s="5"/>
+      <c r="J330" s="5"/>
+    </row>
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A331" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B331" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C331" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D331" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E331" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F331" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G331" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H331" s="6">
+        <v>44002</v>
+      </c>
+      <c r="I331" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J331" s="5"/>
+    </row>
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A332" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B332" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C332" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D332" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E332" s="5">
+        <v>1</v>
+      </c>
+      <c r="F332" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G332" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H332" s="4">
         <v>44005</v>
       </c>
-      <c r="I315" s="5" t="s">
+      <c r="I332" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J315" s="5" t="s">
+      <c r="J332" s="5" t="s">
         <v>270</v>
       </c>
     </row>
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A333" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B333" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C333" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D333" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E333" s="5">
+        <v>1</v>
+      </c>
+      <c r="F333" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G333" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H333" s="6">
+        <v>44005</v>
+      </c>
+      <c r="I333" s="5"/>
+      <c r="J333" s="5"/>
+    </row>
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A334" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B334" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C334" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D334" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E334" s="5">
+        <v>1</v>
+      </c>
+      <c r="F334" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G334" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H334" s="6">
+        <v>44005</v>
+      </c>
+      <c r="I334" s="5"/>
+      <c r="J334" s="5"/>
+    </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A335" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B335" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C335" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D335" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E335" s="5">
+        <v>1</v>
+      </c>
+      <c r="F335" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G335" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H335" s="6">
+        <v>44005</v>
+      </c>
+      <c r="I335" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J335" s="5"/>
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A336" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B336" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C336" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D336" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E336" s="5">
+        <v>2</v>
+      </c>
+      <c r="F336" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G336" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H336" s="6">
+        <v>44006</v>
+      </c>
+      <c r="I336" s="5"/>
+      <c r="J336" s="5"/>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A337" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B337" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C337" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D337" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E337" s="5">
+        <v>1</v>
+      </c>
+      <c r="F337" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G337" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H337" s="6">
+        <v>44006</v>
+      </c>
+      <c r="I337" s="5"/>
+      <c r="J337" s="5"/>
+    </row>
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A338" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B338" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C338" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D338" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E338" s="5">
+        <v>1</v>
+      </c>
+      <c r="F338" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="G338" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H338" s="6">
+        <v>44007</v>
+      </c>
+      <c r="I338" s="5"/>
+      <c r="J338" s="5"/>
+    </row>
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A339" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B339" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C339" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D339" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E339" s="5">
+        <v>3</v>
+      </c>
+      <c r="F339" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G339" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H339" s="6">
+        <v>44007</v>
+      </c>
+      <c r="I339" s="5"/>
+      <c r="J339" s="5"/>
+    </row>
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A340" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B340" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C340" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D340" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E340" s="5">
+        <v>2</v>
+      </c>
+      <c r="F340" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G340" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H340" s="6">
+        <v>44007</v>
+      </c>
+      <c r="I340" s="5"/>
+      <c r="J340" s="5"/>
+    </row>
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A341" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B341" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C341" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D341" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E341" s="5">
+        <v>2</v>
+      </c>
+      <c r="F341" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G341" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H341" s="6">
+        <v>44007</v>
+      </c>
+      <c r="I341" s="5"/>
+      <c r="J341" s="5"/>
+    </row>
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A342" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B342" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C342" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D342" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E342" s="5">
+        <v>1</v>
+      </c>
+      <c r="F342" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="G342" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H342" s="6">
+        <v>44009</v>
+      </c>
+      <c r="I342" s="5"/>
+      <c r="J342" s="5"/>
+    </row>
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A343" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B343" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C343" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D343" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E343" s="5">
+        <v>1</v>
+      </c>
+      <c r="F343" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G343" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H343" s="6">
+        <v>44009</v>
+      </c>
+      <c r="I343" s="5"/>
+      <c r="J343" s="5"/>
+    </row>
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A344" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B344" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C344" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D344" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E344" s="5">
+        <v>1</v>
+      </c>
+      <c r="F344" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G344" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H344" s="6">
+        <v>44009</v>
+      </c>
+      <c r="I344" s="5"/>
+      <c r="J344" s="5"/>
+    </row>
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A345" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B345" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C345" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D345" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E345" s="5">
+        <v>1</v>
+      </c>
+      <c r="F345" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="G345" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H345" s="6">
+        <v>44009</v>
+      </c>
+      <c r="I345" s="5"/>
+      <c r="J345" s="5"/>
+    </row>
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A346" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B346" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C346" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D346" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E346" s="5">
+        <v>2</v>
+      </c>
+      <c r="F346" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G346" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H346" s="6">
+        <v>44011</v>
+      </c>
+      <c r="I346" s="5"/>
+      <c r="J346" s="5"/>
+    </row>
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A347" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B347" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C347" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D347" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E347" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F347" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G347" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H347" s="6">
+        <v>44015</v>
+      </c>
+      <c r="I347" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J347" s="5"/>
+    </row>
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A348" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B348" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C348" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D348" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E348" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F348" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G348" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H348" s="6">
+        <v>44015</v>
+      </c>
+      <c r="I348" s="5"/>
+      <c r="J348" s="5"/>
+    </row>
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A349" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B349" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C349" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D349" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E349" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F349" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G349" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H349" s="6">
+        <v>44015</v>
+      </c>
+      <c r="I349" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J349" s="5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A350" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B350" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C350" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D350" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E350" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F350" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G350" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H350" s="6">
+        <v>44015</v>
+      </c>
+      <c r="I350" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J350" s="5"/>
+    </row>
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A351" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B351" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C351" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D351" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E351" s="5">
+        <v>1</v>
+      </c>
+      <c r="F351" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G351" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H351" s="6">
+        <v>44015</v>
+      </c>
+      <c r="I351" s="5"/>
+      <c r="J351" s="5"/>
+    </row>
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A352" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B352" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C352" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D352" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E352" s="5">
+        <v>1</v>
+      </c>
+      <c r="F352" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G352" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H352" s="6">
+        <v>44015</v>
+      </c>
+      <c r="I352" s="5"/>
+      <c r="J352" s="5"/>
+    </row>
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A353" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B353" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C353" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D353" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E353" s="5">
+        <v>16</v>
+      </c>
+      <c r="F353" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="G353" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H353" s="6">
+        <v>44015</v>
+      </c>
+      <c r="I353" s="5"/>
+      <c r="J353" s="5"/>
+    </row>
+    <row r="354" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A354" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B354" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C354" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D354" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E354" s="5">
+        <v>17</v>
+      </c>
+      <c r="F354" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G354" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H354" s="6">
+        <v>44015</v>
+      </c>
+    </row>
+    <row r="355" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A355" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B355" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C355" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D355" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E355" s="5">
+        <v>16</v>
+      </c>
+      <c r="F355" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G355" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H355" s="6">
+        <v>44015</v>
+      </c>
+    </row>
+    <row r="356" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A356" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B356" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C356" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D356" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E356" s="5">
+        <v>24</v>
+      </c>
+      <c r="F356" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G356" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H356" s="6">
+        <v>44015</v>
+      </c>
+    </row>
+    <row r="357" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A357" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B357" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C357" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D357" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E357" s="5">
+        <v>1</v>
+      </c>
+      <c r="F357" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G357" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H357" s="4">
+        <v>44021</v>
+      </c>
+      <c r="I357" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J357" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="358" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A358" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B358" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C358" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D358" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E358" s="5">
+        <v>6</v>
+      </c>
+      <c r="F358" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G358" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H358" s="4">
+        <v>44021</v>
+      </c>
+      <c r="I358" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J358" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A359" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B359" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C359" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D359" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E359" s="5">
+        <v>1</v>
+      </c>
+      <c r="F359">
+        <v>398</v>
+      </c>
+      <c r="G359" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H359" s="4">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A360" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B360" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C360" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D360" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E360" s="5">
+        <v>1</v>
+      </c>
+      <c r="F360">
+        <v>399</v>
+      </c>
+      <c r="G360" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H360" s="4">
+        <v>44021</v>
+      </c>
+    </row>
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A361" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B361" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C361" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D361" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E361" s="5">
+        <v>1</v>
+      </c>
+      <c r="F361" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G361" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H361" s="4">
+        <v>44025</v>
+      </c>
+      <c r="I361" t="s">
+        <v>17</v>
+      </c>
+      <c r="J361" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A362" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B362" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C362" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D362" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E362" s="5">
+        <v>1</v>
+      </c>
+      <c r="F362">
+        <v>400</v>
+      </c>
+      <c r="G362" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H362" s="4">
+        <v>44028</v>
+      </c>
+    </row>
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A363" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B363" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C363" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D363" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E363" s="5">
+        <v>6</v>
+      </c>
+      <c r="F363" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G363" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H363" s="4">
+        <v>44029</v>
+      </c>
+    </row>
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A364" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B364" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C364" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D364" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E364" s="5">
+        <v>1</v>
+      </c>
+      <c r="F364" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G364" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H364" s="4">
+        <v>44029</v>
+      </c>
+    </row>
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A365" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B365" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C365" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D365" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E365" s="5">
+        <v>1</v>
+      </c>
+      <c r="F365">
+        <v>402</v>
+      </c>
+      <c r="G365" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H365" s="4">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A366" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B366" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C366" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D366" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E366" s="5">
+        <v>1</v>
+      </c>
+      <c r="F366">
+        <v>403</v>
+      </c>
+      <c r="G366" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H366" s="4">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A367" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B367" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C367" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D367" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E367" s="5">
+        <v>1</v>
+      </c>
+      <c r="F367">
+        <v>401</v>
+      </c>
+      <c r="G367" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H367" s="4">
+        <v>44032</v>
+      </c>
+    </row>
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A368" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B368" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C368" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D368" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E368" s="5">
+        <v>1</v>
+      </c>
+      <c r="F368" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G368" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H368" s="4">
+        <v>44033</v>
+      </c>
+      <c r="I368" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J368" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A369" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B369" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C369" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D369" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E369" s="5">
+        <v>1</v>
+      </c>
+      <c r="F369" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G369" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H369" s="4">
+        <v>44033</v>
+      </c>
+      <c r="I369" t="s">
+        <v>15</v>
+      </c>
+      <c r="J369" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A370" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B370" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C370" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D370" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E370" s="5">
+        <v>1</v>
+      </c>
+      <c r="F370" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G370" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H370" s="4">
+        <v>44033</v>
+      </c>
+      <c r="I370" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A371" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B371" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C371" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D371" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E371" s="5">
+        <v>1</v>
+      </c>
+      <c r="F371" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G371" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H371" s="4">
+        <v>44033</v>
+      </c>
+      <c r="I371" t="s">
+        <v>27</v>
+      </c>
+      <c r="J371" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A372" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B372" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C372" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D372" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="E372" s="5">
+        <v>1</v>
+      </c>
+      <c r="F372" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G372" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H372" s="4">
+        <v>44033</v>
+      </c>
+    </row>
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A373" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B373" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C373" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D373" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E373" s="5">
+        <v>1</v>
+      </c>
+      <c r="F373" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G373" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H373" s="4">
+        <v>44035</v>
+      </c>
+      <c r="I373" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J373" s="5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A374" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B374" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C374" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D374" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E374" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F374" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G374" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H374" s="6">
+        <v>44036</v>
+      </c>
+      <c r="I374" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J374" s="5"/>
+    </row>
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A375" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B375" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C375" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D375" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E375" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F375" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G375" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H375" s="6">
+        <v>44037</v>
+      </c>
+      <c r="I375" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J375" s="5"/>
+    </row>
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A376" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B376" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C376" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D376" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E376" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F376" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G376" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H376" s="6">
+        <v>44039</v>
+      </c>
+      <c r="I376" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J376" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A377" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B377" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C377" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D377" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E377" s="5">
+        <v>1</v>
+      </c>
+      <c r="F377" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G377" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H377" s="4">
+        <v>44039</v>
+      </c>
+      <c r="I377" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J377" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A378" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B378" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C378" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D378" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E378" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F378" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G378" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H378" s="6">
+        <v>44040</v>
+      </c>
+      <c r="I378" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J378" s="5"/>
+    </row>
+    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A379" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B379" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C379" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D379" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E379" s="5">
+        <v>1</v>
+      </c>
+      <c r="F379" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G379" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H379" s="4">
+        <v>44040</v>
+      </c>
+      <c r="I379" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J379" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A380" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B380" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C380" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D380" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E380" s="5">
+        <v>1</v>
+      </c>
+      <c r="F380" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G380" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H380" s="4">
+        <v>44040</v>
+      </c>
+      <c r="I380" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J380" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A381" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B381" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C381" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D381" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E381" s="5">
+        <v>1</v>
+      </c>
+      <c r="F381" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G381" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H381" s="4">
+        <v>44040</v>
+      </c>
+      <c r="I381" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J381" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A382" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B382" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C382" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D382" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E382" s="5">
+        <v>1</v>
+      </c>
+      <c r="F382" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G382" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H382" s="4">
+        <v>44040</v>
+      </c>
+      <c r="I382" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J382" s="5" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A383" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B383" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C383" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D383" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E383" s="5">
+        <v>1</v>
+      </c>
+      <c r="F383" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G383" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H383" s="4">
+        <v>44040</v>
+      </c>
+      <c r="I383" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J383" s="5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A384" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B384" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C384" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D384" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E384" s="5">
+        <v>2</v>
+      </c>
+      <c r="F384" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G384" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H384" s="6">
+        <v>44041</v>
+      </c>
+      <c r="I384" s="5"/>
+      <c r="J384" s="5"/>
+    </row>
+    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A385" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B385" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C385" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D385" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E385" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F385" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G385" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H385" s="6">
+        <v>44041</v>
+      </c>
+      <c r="I385" s="5"/>
+      <c r="J385" s="5"/>
+    </row>
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A386" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B386" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C386" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D386" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E386" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F386" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G386" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H386" s="6">
+        <v>44041</v>
+      </c>
+      <c r="I386" s="5"/>
+      <c r="J386" s="5"/>
+    </row>
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A387" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B387" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C387" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D387" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E387" s="5">
+        <v>1</v>
+      </c>
+      <c r="F387" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G387" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H387" s="6">
+        <v>44041</v>
+      </c>
+      <c r="I387" s="5"/>
+      <c r="J387" s="5"/>
+    </row>
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A388" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B388" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C388" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D388" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E388" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F388" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G388" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H388" s="6">
+        <v>44041</v>
+      </c>
+      <c r="I388" s="5"/>
+      <c r="J388" s="5"/>
+    </row>
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A389" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B389" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C389" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D389" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E389" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="F389" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G389" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H389" s="6">
+        <v>44041</v>
+      </c>
+      <c r="I389" s="5"/>
+      <c r="J389" s="5"/>
+    </row>
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A390" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B390" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C390" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D390" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E390" s="5">
+        <v>25</v>
+      </c>
+      <c r="F390" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G390" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H390" s="6">
+        <v>44041</v>
+      </c>
+      <c r="I390" s="5"/>
+      <c r="J390" s="5"/>
+    </row>
+    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A391" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B391" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C391" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D391" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E391" s="5">
+        <v>1</v>
+      </c>
+      <c r="F391" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G391" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H391" s="4">
+        <v>44042</v>
+      </c>
+    </row>
+    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A392" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B392" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C392" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D392" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E392" s="5">
+        <v>1</v>
+      </c>
+      <c r="F392" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G392" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H392" s="6">
+        <v>44042</v>
+      </c>
+      <c r="I392" s="5"/>
+      <c r="J392" s="5"/>
+    </row>
+    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A393" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B393" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C393" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D393" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E393" s="5">
+        <v>1</v>
+      </c>
+      <c r="F393" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G393" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H393" s="4">
+        <v>44043</v>
+      </c>
+    </row>
+    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A394" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B394" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C394" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D394" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E394" s="5">
+        <v>1</v>
+      </c>
+      <c r="F394" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G394" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H394" s="4">
+        <v>44043</v>
+      </c>
+    </row>
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A395" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B395" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C395" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D395" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E395" s="5">
+        <v>1</v>
+      </c>
+      <c r="F395" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G395" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H395" s="6">
+        <v>44043</v>
+      </c>
+      <c r="I395" s="5"/>
+      <c r="J395" s="5"/>
+    </row>
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A396" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B396" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C396" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D396" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E396" s="5">
+        <v>1</v>
+      </c>
+      <c r="F396" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G396" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H396" s="6">
+        <v>44043</v>
+      </c>
+      <c r="I396" s="5"/>
+      <c r="J396" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J309" xr:uid="{666A33B2-D072-48D0-88E3-92275EF5620C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A155:J225">
-      <sortCondition ref="D1:D225"/>
+  <autoFilter ref="A1:J396" xr:uid="{666A33B2-D072-48D0-88E3-92275EF5620C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J396">
+      <sortCondition ref="H1:H396"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J315">
-    <sortCondition ref="H2:H315"/>
-    <sortCondition ref="C2:C315"/>
-    <sortCondition ref="D2:D315"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J388">
+    <sortCondition ref="H2:H388"/>
+    <sortCondition ref="C2:C388"/>
+    <sortCondition ref="D2:D388"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10803,11 +13384,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4D434A2C-7767-4A66-A150-E372D25D3050}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D4698F7A-0802-4195-8585-1B0866AABCC3}">
           <x14:formula1>
-            <xm:f>Config!$B$2:$B$103</xm:f>
+            <xm:f>Config!$D$2:$D$16</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>I2:I300 I302:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C7C869D3-BE0F-4D79-B0ED-E3C1B1A79587}">
           <x14:formula1>
@@ -10821,15 +13402,15 @@
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D4698F7A-0802-4195-8585-1B0866AABCC3}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4D434A2C-7767-4A66-A150-E372D25D3050}">
           <x14:formula1>
-            <xm:f>Config!$D$2:$D$16</xm:f>
+            <xm:f>Config!$B$2:$B$106</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I300 I302:I1048576</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF95E1C6-5B3F-419D-ADFD-AA23C2C80F28}">
           <x14:formula1>
-            <xm:f>Config!$C$2:$C$44</xm:f>
+            <xm:f>Config!$C$2:$C$45</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>

</xml_diff>